<commit_message>
Added Diagram related files, and Datasheet update
</commit_message>
<xml_diff>
--- a/reference/Instructions.xlsx
+++ b/reference/Instructions.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeeva\Dropbox\JEEVAHA\University\Imperial\Work\Year 2\Instr Arch and Compilers\Coursework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeeva\Dropbox\JEEVAHA\University\Imperial\Work\Year 2\Instr Arch and Compilers\Coursework\jl7719\AM04_CPU\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17322F4-318B-4C44-B67B-3B3F4A962439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4FB052-5200-4C48-A8AC-FD8266BD7488}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23028" yWindow="2808" windowWidth="30960" windowHeight="12204" xr2:uid="{FF8D8181-7B5F-469C-8171-05828C14D0C2}"/>
+    <workbookView xWindow="0" yWindow="2808" windowWidth="30960" windowHeight="12204" xr2:uid="{FF8D8181-7B5F-469C-8171-05828C14D0C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1051,9 +1050,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3ECEA77-E1C3-40D6-8874-060C332F3FAA}">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B18" sqref="B18"/>
+      <selection pane="topRight" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>